<commit_message>
Update files: A_model.xlsx, trucks.csv, analisis_explorativoLDHR.ipynb, and add new data files
</commit_message>
<xml_diff>
--- a/MY_DATA/A_model.xlsx
+++ b/MY_DATA/A_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dishi\OneDrive\Desktop\TFG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dishi\TFG-LDHR\MY_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CB52F5-A0E5-4E57-A9F9-C400E41A446D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDA20D2-087D-4DF7-80A9-92ECE2DCD5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yt_growth_rate" sheetId="13" r:id="rId1"/>
@@ -21,10 +21,10 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="2" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="29" r:id="rId6"/>
+    <pivotCache cacheId="30" r:id="rId7"/>
+    <pivotCache cacheId="31" r:id="rId8"/>
+    <pivotCache cacheId="32" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -17053,7 +17053,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8D64F192-3E27-44A8-B28E-C72A535E739F}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8D64F192-3E27-44A8-B28E-C72A535E739F}" name="PivotTable10" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E258" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="14" showAll="0"/>
@@ -18120,7 +18120,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81C5CB25-CAE9-412B-8EA9-1F2A042C6F55}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81C5CB25-CAE9-412B-8EA9-1F2A042C6F55}" name="PivotTable12" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E262" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="14" showAll="0"/>
@@ -19198,7 +19198,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{681B1EEB-2599-496A-B701-A8861637084C}" name="PivotTable13" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{681B1EEB-2599-496A-B701-A8861637084C}" name="PivotTable13" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E343" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="14" showAll="0"/>
@@ -20600,7 +20600,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CE71E39-0DCB-4DDF-B37A-37B5DE7AA60B}" name="PivotTable14" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CE71E39-0DCB-4DDF-B37A-37B5DE7AA60B}" name="PivotTable14" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E130" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="164" showAll="0"/>
@@ -21150,9 +21150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -21190,7 +21190,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -21296,7 +21296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -21438,7 +21438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -22487,7 +22487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F768"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+    <sheetView zoomScale="118" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -33271,7 +33271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304C9B1C-3B48-45E7-9066-664C4734FA58}">
   <dimension ref="A1:F781"/>
   <sheetViews>
-    <sheetView zoomScale="180" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="103" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -58593,8 +58593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32948DD1-DF60-42DF-8379-F80AE75401D3}">
   <dimension ref="A1:F384"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="152" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>